<commit_message>
falta o ajuste de pesos
</commit_message>
<xml_diff>
--- a/dados/previsoes/previsao_rodada-27.xlsx
+++ b/dados/previsoes/previsao_rodada-27.xlsx
@@ -687,109 +687,109 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>0.3992679288412299</v>
+        <v>0.4103084890224243</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3869091940498399</v>
+        <v>0.362725602719507</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2138228771089302</v>
+        <v>0.2269659082580686</v>
       </c>
       <c r="N2" t="n">
-        <v>0.001959301241158507</v>
+        <v>0.1746273974089039</v>
       </c>
       <c r="O2" t="n">
-        <v>0.01221657118434385</v>
+        <v>0.3047423991504375</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0380861830654214</v>
+        <v>0.2659030920059666</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.07915790874566365</v>
+        <v>0.1546758935534708</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1233907025985701</v>
+        <v>0.06748125378895869</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1538723367408601</v>
+        <v>0.02355231708478556</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1599032957607333</v>
+        <v>0.006850194299850672</v>
       </c>
       <c r="U2" t="n">
-        <v>0.1424319733583861</v>
+        <v>0.001707754155875252</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1110108992498797</v>
+        <v>0.000372525378564981</v>
       </c>
       <c r="W2" t="n">
-        <v>0.07690794863412594</v>
+        <v>7.223270122734607e-05</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04795339325029553</v>
+        <v>1.260533398295713e-05</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.02718158484569452</v>
+        <v>1.99977977893958e-06</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.01412347759476245</v>
+        <v>2.90818096438967e-07</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.006774018982748724</v>
+        <v>3.903899024224559e-08</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.003016938727528701</v>
+        <v>4.866212176552516e-09</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.001254074529205294</v>
+        <v>5.661353622861605e-10</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.002100947576507217</v>
+        <v>0.1957460509155415</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.01295311245589199</v>
+        <v>0.3192495002256387</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.039930344805157</v>
+        <v>0.2603379299802466</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.0820617408461016</v>
+        <v>0.1415315977806226</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.1264851833277249</v>
+        <v>0.05770728406303247</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.155965510226762</v>
+        <v>0.01882339031651889</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.1602640966865078</v>
+        <v>0.005116627660340079</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.1411552774862973</v>
+        <v>0.001192128281781529</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.1087842578432114</v>
+        <v>0.0002430357830870199</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.07452165029566002</v>
+        <v>4.404178663833926e-05</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.04594533092934719</v>
+        <v>7.182938459075523e-06</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.02575180166778957</v>
+        <v>1.064992813850527e-06</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.01323077527312909</v>
+        <v>1.447446925814684e-07</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.006274814055987198</v>
+        <v>1.815919167906824e-08</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.002763323593868774</v>
+        <v>2.115464267871911e-09</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.001135793571232528</v>
+        <v>2.300126131466461e-10</v>
       </c>
     </row>
     <row r="3">
@@ -824,109 +824,109 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0.3445676239433939</v>
+        <v>0.3741074289656309</v>
       </c>
       <c r="L3" t="n">
-        <v>0.4858160912515388</v>
+        <v>0.3893121292810714</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1696162848050673</v>
+        <v>0.2365804417532977</v>
       </c>
       <c r="N3" t="n">
-        <v>0.005991996684547221</v>
+        <v>0.2113288893302999</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03066302790552696</v>
+        <v>0.3284768701520276</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0784564252813978</v>
+        <v>0.2552823103523546</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1338291549223477</v>
+        <v>0.1322651382803584</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1712120069483617</v>
+        <v>0.05139623691564073</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1752296879722186</v>
+        <v>0.01597744169587249</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1494513736415985</v>
+        <v>0.004139061833846032</v>
       </c>
       <c r="U3" t="n">
-        <v>0.1092560122097014</v>
+        <v>0.0009190725554817676</v>
       </c>
       <c r="V3" t="n">
-        <v>0.06988739162423738</v>
+        <v>0.0001785688633390217</v>
       </c>
       <c r="W3" t="n">
-        <v>0.03973743186001139</v>
+        <v>3.08396292317875e-05</v>
       </c>
       <c r="X3" t="n">
-        <v>0.02033495754695289</v>
+        <v>4.793525825460385e-06</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.009460063656515676</v>
+        <v>6.773424740631977e-07</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.00403418942464642</v>
+        <v>8.773502154484744e-08</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.001588021610214309</v>
+        <v>1.049000168960086e-08</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.00058045939695047</v>
+        <v>1.164644676365099e-09</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.0001980268417328358</v>
+        <v>1.206835592754517e-10</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.003053744141402952</v>
+        <v>0.2039976250439873</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.01768541367565505</v>
+        <v>0.3242841977964455</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.05121153613336971</v>
+        <v>0.257748689274713</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.09886193904338299</v>
+        <v>0.1365764706272319</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.1431369335314028</v>
+        <v>0.05427709171328793</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.1657922710318885</v>
+        <v>0.01725628241130003</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.1600278631550209</v>
+        <v>0.004571899384850442</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.1323976089902273</v>
+        <v>0.001038243686907491</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.09584572152400683</v>
+        <v>0.0002063051108152735</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.06167551684838159</v>
+        <v>3.643914282913409e-05</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.03571867774823935</v>
+        <v>5.792537142620075e-06</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.01880551643176127</v>
+        <v>8.370989881045876e-07</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.009075835053621325</v>
+        <v>1.108909861798553e-07</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.004043205524429845</v>
+        <v>1.35598088791615e-08</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.001672554808696113</v>
+        <v>1.539664894104187e-09</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.0006457607954325288</v>
+        <v>1.631682378499141e-10</v>
       </c>
     </row>
     <row r="4">
@@ -961,109 +961,109 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0.2370583711053921</v>
+        <v>0.3274009040957783</v>
       </c>
       <c r="L4" t="n">
-        <v>0.560072196410673</v>
+        <v>0.4414379664870582</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2028694324839349</v>
+        <v>0.2311611294171635</v>
       </c>
       <c r="N4" t="n">
-        <v>0.006492958239877237</v>
+        <v>0.2282091199810196</v>
       </c>
       <c r="O4" t="n">
-        <v>0.03270527113419646</v>
+        <v>0.337177349350874</v>
       </c>
       <c r="P4" t="n">
-        <v>0.08236883100464291</v>
+        <v>0.2490885660589219</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1382982841559437</v>
+        <v>0.1226755274056571</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1741533948630402</v>
+        <v>0.04531305449613515</v>
       </c>
       <c r="S4" t="n">
-        <v>0.1754434200101739</v>
+        <v>0.01338994305509725</v>
       </c>
       <c r="T4" t="n">
-        <v>0.147285834082615</v>
+        <v>0.003297257582323568</v>
       </c>
       <c r="U4" t="n">
-        <v>0.1059834573292892</v>
+        <v>0.0006959535133060654</v>
       </c>
       <c r="V4" t="n">
-        <v>0.06673032498510797</v>
+        <v>0.000128533294871982</v>
       </c>
       <c r="W4" t="n">
-        <v>0.03734701316038967</v>
+        <v>2.110078085489393e-05</v>
       </c>
       <c r="X4" t="n">
-        <v>0.01881182885115924</v>
+        <v>3.117625342264379e-06</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.008614170787062825</v>
+        <v>4.187517488988109e-07</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.003615824774816495</v>
+        <v>5.155856053630666e-08</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.001401003331552832</v>
+        <v>5.859800458936802e-09</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.0005040646907174197</v>
+        <v>6.184152458291845e-10</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.0001692661677470835</v>
+        <v>6.09136080697084e-11</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.001068854151069696</v>
+        <v>0.1744684430155444</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.007312210912410558</v>
+        <v>0.3046238897495054</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.02501203198493712</v>
+        <v>0.2659383914999777</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.05703717170354252</v>
+        <v>0.1547771540653005</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.09755021976718757</v>
+        <v>0.06756066871005652</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.1334714901515437</v>
+        <v>0.02359233949798185</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.1521834832508996</v>
+        <v>0.006865415603674348</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.1487303985169809</v>
+        <v>0.001712441983195696</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.1271862070651356</v>
+        <v>0.0003737429022085048</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.09667802460118941</v>
+        <v>7.250659627049146e-05</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.06613906170188193</v>
+        <v>1.265973433742754e-05</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.04113349440861015</v>
+        <v>2.00945822032957e-06</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.02345009578553551</v>
+        <v>2.923780793753514e-07</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.01234046515560313</v>
+        <v>3.926888142563744e-08</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.006030228318048816</v>
+        <v>4.897422462698793e-09</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.002750253703459592</v>
+        <v>5.700636953969515e-10</v>
       </c>
     </row>
     <row r="5">
@@ -1098,109 +1098,109 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0.4060325426586354</v>
+        <v>0.3790063592041725</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4301407871193546</v>
+        <v>0.3689697158364057</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1638266702220101</v>
+        <v>0.2520239249594218</v>
       </c>
       <c r="N5" t="n">
-        <v>0.005226403797795706</v>
+        <v>0.2420846928811411</v>
       </c>
       <c r="O5" t="n">
-        <v>0.02745969200298664</v>
+        <v>0.3433893038307004</v>
       </c>
       <c r="P5" t="n">
-        <v>0.07213704815698614</v>
+        <v>0.2435433082983641</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1263367828072593</v>
+        <v>0.1151527675347647</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1659443701039097</v>
+        <v>0.04083511870095376</v>
       </c>
       <c r="S5" t="n">
-        <v>0.174375401097208</v>
+        <v>0.01158465891889269</v>
       </c>
       <c r="T5" t="n">
-        <v>0.1526956518057438</v>
+        <v>0.002738743972843018</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1146096882293123</v>
+        <v>0.0005549742441742639</v>
       </c>
       <c r="V5" t="n">
-        <v>0.0752703690026444</v>
+        <v>9.840162603988808e-05</v>
       </c>
       <c r="W5" t="n">
-        <v>0.04394143510379843</v>
+        <v>1.550883584468714e-05</v>
       </c>
       <c r="X5" t="n">
-        <v>0.0230869699472596</v>
+        <v>2.199878183353991e-06</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.01102724321560765</v>
+        <v>2.836778202416373e-07</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.004828123920669914</v>
+        <v>3.35323174318495e-08</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.001951316680325935</v>
+        <v>3.658808252889589e-09</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.0007323057131100256</v>
+        <v>3.707072228840167e-10</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.0002565038359328455</v>
+        <v>3.50557467240483e-11</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.004678219413788816</v>
+        <v>0.2475144979072078</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.02509788792014132</v>
+        <v>0.345601058244937</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.06732304775994105</v>
+        <v>0.241278980564601</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.1203924084265277</v>
+        <v>0.1122981639734721</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.1614714331385821</v>
+        <v>0.03920009195051805</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.173253606672313</v>
+        <v>0.01094690886872964</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.1549129137040745</v>
+        <v>0.002547502820731856</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.1187260915695446</v>
+        <v>0.0005081489760750198</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.07961827663069122</v>
+        <v>8.869017035491288e-05</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.04745990364012224</v>
+        <v>1.375965044011854e-05</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.0254614680694467</v>
+        <v>1.921240894328599e-06</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.01241787672863359</v>
+        <v>2.438729087634868e-07</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.005551657777863948</v>
+        <v>2.83763631553445e-08</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0.002291057153219905</v>
+        <v>3.047809388183264e-09</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.0008779392720088359</v>
+        <v>3.039724249318445e-10</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.0003140001141548694</v>
+        <v>2.829549854573479e-11</v>
       </c>
     </row>
     <row r="6">
@@ -1235,109 +1235,109 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0.4269534526294731</v>
+        <v>0.3596950327332304</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4013053980747178</v>
+        <v>0.4037159281887885</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1717411492958092</v>
+        <v>0.236589039077981</v>
       </c>
       <c r="N6" t="n">
-        <v>0.003809214747583167</v>
+        <v>0.2192635895907709</v>
       </c>
       <c r="O6" t="n">
-        <v>0.02121859161881956</v>
+        <v>0.3327282582864101</v>
       </c>
       <c r="P6" t="n">
-        <v>0.05909730221588271</v>
+        <v>0.2524543497370708</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1097305354328279</v>
+        <v>0.1276981983824693</v>
       </c>
       <c r="R6" t="n">
-        <v>0.1528088840974927</v>
+        <v>0.04844488682937705</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1702392499372437</v>
+        <v>0.0147028358403737</v>
       </c>
       <c r="T6" t="n">
-        <v>0.1580481963377703</v>
+        <v>0.003718544857484826</v>
       </c>
       <c r="U6" t="n">
-        <v>0.1257687084911246</v>
+        <v>0.0008061171331989825</v>
       </c>
       <c r="V6" t="n">
-        <v>0.08757168605395331</v>
+        <v>0.0001529083956692992</v>
       </c>
       <c r="W6" t="n">
-        <v>0.05420037598531453</v>
+        <v>2.578172603596073e-05</v>
       </c>
       <c r="X6" t="n">
-        <v>0.03019141003663647</v>
+        <v>3.912327083385336e-06</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.01528874399233102</v>
+        <v>5.397164285362056e-07</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.00709694859777813</v>
+        <v>6.825077051878364e-08</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.003040950876606857</v>
+        <v>7.966863446377979e-09</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.001209936187814618</v>
+        <v>8.635400900240674e-10</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.0004493164349311729</v>
+        <v>8.736035948040248e-11</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.004307192556023231</v>
+        <v>0.1979703969858633</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.0234632977804659</v>
+        <v>0.3206403322284874</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.06390779325212113</v>
+        <v>0.2596605962732304</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.1160452401468225</v>
+        <v>0.1401853696702627</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.1580382110943107</v>
+        <v>0.05676237986714762</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.1721816500826038</v>
+        <v>0.01838689886547177</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.1563256992295596</v>
+        <v>0.004963352644837987</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.1216541993107865</v>
+        <v>0.001148404772515874</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.08283843441946578</v>
+        <v>0.0002324999680498727</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.05013997785668949</v>
+        <v>4.184063663257207e-05</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.02731359733412214</v>
+        <v>6.776667539580328e-06</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.01352636125758467</v>
+        <v>9.977951544893222e-07</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.006140369431379935</v>
+        <v>1.346722265477054e-07</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.002573036301427832</v>
+        <v>1.677847881829834e-08</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.001001181100070206</v>
+        <v>1.941075572227365e-09</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.0003635935314798275</v>
+        <v>2.095892873667126e-10</v>
       </c>
     </row>
     <row r="7">
@@ -1372,109 +1372,109 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>0.3002999666905673</v>
+        <v>0.3362439269272987</v>
       </c>
       <c r="L7" t="n">
-        <v>0.5038946264215464</v>
+        <v>0.4413954956665697</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1958054068878863</v>
+        <v>0.2223605774061316</v>
       </c>
       <c r="N7" t="n">
-        <v>0.004681909940790188</v>
+        <v>0.2011644635979934</v>
       </c>
       <c r="O7" t="n">
-        <v>0.02511399501626318</v>
+        <v>0.3225938673724233</v>
       </c>
       <c r="P7" t="n">
-        <v>0.06735635175101677</v>
+        <v>0.258661001563038</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.1204342603468367</v>
+        <v>0.1382657276873647</v>
       </c>
       <c r="R7" t="n">
-        <v>0.1615038228195461</v>
+        <v>0.05543185290030297</v>
       </c>
       <c r="S7" t="n">
-        <v>0.1732628885515462</v>
+        <v>0.01777846393234076</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1548984415411637</v>
+        <v>0.004751687030349623</v>
       </c>
       <c r="U7" t="n">
-        <v>0.1186975504224356</v>
+        <v>0.001088565664309338</v>
       </c>
       <c r="V7" t="n">
-        <v>0.07958743673657095</v>
+        <v>0.0002182074068013244</v>
       </c>
       <c r="W7" t="n">
-        <v>0.04743454688926153</v>
+        <v>3.888049829164147e-05</v>
       </c>
       <c r="X7" t="n">
-        <v>0.02544412406989953</v>
+        <v>6.23500298458908e-06</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.01240759381545727</v>
+        <v>9.089684809506809e-07</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.005546245250085225</v>
+        <v>1.214709481754786e-07</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.002288487084103009</v>
+        <v>1.498421213111386e-08</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.000876825513393631</v>
+        <v>1.716369231440924e-09</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.0003135556763797062</v>
+        <v>1.834950296576084e-10</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.001574258678666799</v>
+        <v>0.1557768905313554</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.01016021954017405</v>
+        <v>0.2896407213191619</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.03278688010535778</v>
+        <v>0.269268911326094</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.07053518891611738</v>
+        <v>0.1668866317703629</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.1138080123690852</v>
+        <v>0.07757435046946798</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.1469027176753447</v>
+        <v>0.02884727092600373</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.1580176416637497</v>
+        <v>0.008939435037076534</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.1456916064032212</v>
+        <v>0.002374480582446916</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.1175361716499278</v>
+        <v>0.000551868016424294</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.08428611327828159</v>
+        <v>0.0001140116695849653</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.05439801137514153</v>
+        <v>2.119853728287404e-05</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.0319166524426588</v>
+        <v>3.583189690296733e-06</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.01716576190216041</v>
+        <v>5.55194485192286e-07</v>
       </c>
       <c r="AQ7" t="n">
-        <v>0.008522102002859343</v>
+        <v>7.940692546539901e-08</v>
       </c>
       <c r="AR7" t="n">
-        <v>0.003928671247260846</v>
+        <v>1.054597979891246e-08</v>
       </c>
       <c r="AS7" t="n">
-        <v>0.001690368633577793</v>
+        <v>1.307230781816758e-09</v>
       </c>
     </row>
     <row r="8">
@@ -1509,109 +1509,109 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>0.4393150446534946</v>
+        <v>0.4141374343938785</v>
       </c>
       <c r="L8" t="n">
-        <v>0.3867619268892489</v>
+        <v>0.3555827390842121</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1739230284572565</v>
+        <v>0.2302798265219095</v>
       </c>
       <c r="N8" t="n">
-        <v>0.003402017121872659</v>
+        <v>0.1805234510570689</v>
       </c>
       <c r="O8" t="n">
-        <v>0.01933497904099347</v>
+        <v>0.3090371186721262</v>
       </c>
       <c r="P8" t="n">
-        <v>0.05494408186721204</v>
+        <v>0.2645194853021565</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.1040894889974767</v>
+        <v>0.150943158338968</v>
       </c>
       <c r="R8" t="n">
-        <v>0.1478952057012358</v>
+        <v>0.06459969392231296</v>
       </c>
       <c r="S8" t="n">
-        <v>0.1681091305573888</v>
+        <v>0.02211757326813094</v>
       </c>
       <c r="T8" t="n">
-        <v>0.1592382009205152</v>
+        <v>0.006310492325492959</v>
       </c>
       <c r="U8" t="n">
-        <v>0.1292874687922494</v>
+        <v>0.00154327109323589</v>
       </c>
       <c r="V8" t="n">
-        <v>0.09184883591889553</v>
+        <v>0.0003302396788276763</v>
       </c>
       <c r="W8" t="n">
-        <v>0.05800138414007046</v>
+        <v>6.281505761810075e-05</v>
       </c>
       <c r="X8" t="n">
-        <v>0.03296442982272705</v>
+        <v>1.075327571118981e-05</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.01703178215874803</v>
+        <v>1.673497680124625e-06</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.008066517090525678</v>
+        <v>2.387376349821668e-07</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.003526548951398331</v>
+        <v>3.143797423184523e-08</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.001431624399367067</v>
+        <v>3.844178422173361e-09</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.0005424316763599027</v>
+        <v>4.387218821317025e-10</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.004388156139766445</v>
+        <v>0.2073996961756615</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.02382262458184745</v>
+        <v>0.3262620067891549</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.06466468191784168</v>
+        <v>0.2566225964572512</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.1170182032397866</v>
+        <v>0.1345649726131913</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.1588184556470757</v>
+        <v>0.05292129016804649</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.1724401924198826</v>
+        <v>0.01665017514536189</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.1560252125645283</v>
+        <v>0.004365419088910379</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.1210052678762812</v>
+        <v>0.0009810390404107641</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.08211487288815905</v>
+        <v>0.0001929099776692946</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.04953211242804984</v>
+        <v>3.371868029842322e-05</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.02689022180468933</v>
+        <v>5.304310711780334e-06</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.01327117065640522</v>
+        <v>7.585682443434338e-07</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.006003928647921808</v>
+        <v>9.944244625620419e-08</v>
       </c>
       <c r="AQ8" t="n">
-        <v>0.002507261919095163</v>
+        <v>1.203335791258919e-08</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.0009722528018689017</v>
+        <v>1.352126068431195e-09</v>
       </c>
       <c r="AS8" t="n">
-        <v>0.0003518807255994748</v>
+        <v>1.418026392686229e-10</v>
       </c>
     </row>
     <row r="9">
@@ -1646,109 +1646,109 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>0.3507026944956574</v>
+        <v>0.4005764513874357</v>
       </c>
       <c r="L9" t="n">
-        <v>0.4374103795170629</v>
+        <v>0.3834075373866053</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2118869259872798</v>
+        <v>0.216016011225959</v>
       </c>
       <c r="N9" t="n">
-        <v>0.002677842913715093</v>
+        <v>0.1539075573271856</v>
       </c>
       <c r="O9" t="n">
-        <v>0.01586017722401715</v>
+        <v>0.2880230851134713</v>
       </c>
       <c r="P9" t="n">
-        <v>0.04696788229975976</v>
+        <v>0.2695036520588996</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.09272624286457343</v>
+        <v>0.1681166596871215</v>
       </c>
       <c r="R9" t="n">
-        <v>0.1372984424905161</v>
+        <v>0.07865351094995143</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1626366968225228</v>
+        <v>0.02943848537684473</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1605425783518279</v>
+        <v>0.0091818789652648</v>
       </c>
       <c r="U9" t="n">
-        <v>0.1358360775927744</v>
+        <v>0.002454713867245113</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1005652839549815</v>
+        <v>0.0005742199029997483</v>
       </c>
       <c r="W9" t="n">
-        <v>0.06618026679195983</v>
+        <v>0.0001193996584470316</v>
       </c>
       <c r="X9" t="n">
-        <v>0.039196875764345</v>
+        <v>2.234448950047386e-05</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.02110482260541236</v>
+        <v>3.801413425150216e-06</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.01041653791219164</v>
+        <v>5.928314164239648e-07</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.004745729554356773</v>
+        <v>8.534050542861863e-08</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.002007695698542971</v>
+        <v>1.140760637914241e-08</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.0007927378021989616</v>
+        <v>1.423215355217365e-09</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.001645004416423942</v>
+        <v>0.1606600573993105</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.01054449839480147</v>
+        <v>0.2937612261369779</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.0337951817295658</v>
+        <v>0.268566000094903</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.07220917584203282</v>
+        <v>0.1636878071701743</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.1157154247055873</v>
+        <v>0.07482433984582587</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.1483474570499125</v>
+        <v>0.02736273119007871</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.1584848351690337</v>
+        <v>0.008338630848856887</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.1451271040764682</v>
+        <v>0.002178127320608547</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.1162833136417342</v>
+        <v>0.0004978285850431631</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.08281971780713304</v>
+        <v>0.0001011402155690475</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.05308754023734867</v>
+        <v>1.849313028905291e-05</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.03093561646553817</v>
+        <v>3.074003082693454e-06</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.01652480660569626</v>
+        <v>4.683921491017489e-07</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.008148016316200253</v>
+        <v>6.587988148602741e-08</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.003730634576730158</v>
+        <v>8.604216468153181e-09</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.001594227545862265</v>
+        <v>1.048833676334164e-09</v>
       </c>
     </row>
     <row r="10">
@@ -1783,109 +1783,109 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0.3490501999302086</v>
+        <v>0.3561540598670802</v>
       </c>
       <c r="L10" t="n">
-        <v>0.481936965572505</v>
+        <v>0.4083679394766216</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1690128344972864</v>
+        <v>0.2354780006562982</v>
       </c>
       <c r="N10" t="n">
-        <v>0.00594562748321664</v>
+        <v>0.2188612619886077</v>
       </c>
       <c r="O10" t="n">
-        <v>0.03047193069548164</v>
+        <v>0.3325196921880944</v>
       </c>
       <c r="P10" t="n">
-        <v>0.07808583391167045</v>
+        <v>0.2526014532864671</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1333992151359394</v>
+        <v>0.1279272490250826</v>
       </c>
       <c r="R10" t="n">
-        <v>0.1709210529052025</v>
+        <v>0.04859051926524163</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1751974705185649</v>
+        <v>0.0147648828874786</v>
       </c>
       <c r="T10" t="n">
-        <v>0.1496507361848474</v>
+        <v>0.003738756894305337</v>
       </c>
       <c r="U10" t="n">
-        <v>0.1095678384643624</v>
+        <v>0.0008114796955089419</v>
       </c>
       <c r="V10" t="n">
-        <v>0.07019325524438767</v>
+        <v>0.0001541118881179436</v>
       </c>
       <c r="W10" t="n">
-        <v>0.0399719329715643</v>
+        <v>2.601609456647582e-05</v>
       </c>
       <c r="X10" t="n">
-        <v>0.02048601219488079</v>
+        <v>3.952670142983629e-06</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.009544804076476709</v>
+        <v>5.45941814431033e-07</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.00407650564975912</v>
+        <v>6.912156832359947e-08</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.001607115066942966</v>
+        <v>8.078276274793709e-09</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.000588330296721516</v>
+        <v>8.766760392593872e-10</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.0002010167424532418</v>
+        <v>8.879660233899933e-11</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.00316100397538063</v>
+        <v>0.1938038665650151</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.01819747500976531</v>
+        <v>0.3180144368654879</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.05238020883715565</v>
+        <v>0.260916316705545</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.1005152739176432</v>
+        <v>0.1427132784582424</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.144663230374123</v>
+        <v>0.05854486250265329</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.1665613545612854</v>
+        <v>0.01921335400592012</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.1598118883972971</v>
+        <v>0.005254559728163965</v>
       </c>
       <c r="AK10" t="n">
-        <v>0.1314307944123097</v>
+        <v>0.001231750342347535</v>
       </c>
       <c r="AL10" t="n">
-        <v>0.09457867719636495</v>
+        <v>0.0002526487206004194</v>
       </c>
       <c r="AM10" t="n">
-        <v>0.06049741468013847</v>
+        <v>4.606371839884764e-05</v>
       </c>
       <c r="AN10" t="n">
-        <v>0.03482754847420481</v>
+        <v>7.558635297725446e-06</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.01822704684814334</v>
+        <v>1.127548170821064e-06</v>
       </c>
       <c r="AP10" t="n">
-        <v>0.008744221564420623</v>
+        <v>1.541836268705543e-07</v>
       </c>
       <c r="AQ10" t="n">
-        <v>0.003872254478390096</v>
+        <v>1.946163413009452e-08</v>
       </c>
       <c r="AR10" t="n">
-        <v>0.001592289182505026</v>
+        <v>2.281054526214564e-09</v>
       </c>
       <c r="AS10" t="n">
-        <v>0.0006111063200727908</v>
+        <v>2.495334702624018e-10</v>
       </c>
     </row>
     <row r="11">
@@ -1920,109 +1920,109 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>0.4356038602026643</v>
+        <v>0.3896445058944634</v>
       </c>
       <c r="L11" t="n">
-        <v>0.3971210158528823</v>
+        <v>0.3656320204026326</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1672751239444533</v>
+        <v>0.244723473702904</v>
       </c>
       <c r="N11" t="n">
-        <v>0.004119639072419866</v>
+        <v>0.2214293708917937</v>
       </c>
       <c r="O11" t="n">
-        <v>0.02262501544918672</v>
+        <v>0.3338383470062968</v>
       </c>
       <c r="P11" t="n">
-        <v>0.06212817616753675</v>
+        <v>0.2516559602798993</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.1137357683452464</v>
+        <v>0.1264698376970331</v>
       </c>
       <c r="R11" t="n">
-        <v>0.1561589177292167</v>
+        <v>0.04766811353084245</v>
       </c>
       <c r="S11" t="n">
-        <v>0.1715246342722193</v>
+        <v>0.0143733815996988</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1570019214509133</v>
+        <v>0.003611675312695985</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1231789913053294</v>
+        <v>0.0007778782987859609</v>
       </c>
       <c r="V11" t="n">
-        <v>0.08456221929598802</v>
+        <v>0.0001465961834652438</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0516016488164345</v>
+        <v>2.455733018632947e-05</v>
       </c>
       <c r="X11" t="n">
-        <v>0.02833957250020837</v>
+        <v>3.702389833505089e-06</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.0141491491756501</v>
+        <v>5.074467258760834e-07</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.006475581822104706</v>
+        <v>6.375440600538531e-08</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.002735679139922842</v>
+        <v>7.393802516068671e-09</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.001073165837324107</v>
+        <v>7.962341607149554e-10</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.0003929210499943958</v>
+        <v>8.002958083126889e-11</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.004933589103408736</v>
+        <v>0.2337816010325194</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.02620568871614263</v>
+        <v>0.3397706811831703</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.0695982282566743</v>
+        <v>0.2469059055156721</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.1232280372132661</v>
+        <v>0.1196150414670399</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.1636372383586276</v>
+        <v>0.0434611662546489</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.1738380088375252</v>
+        <v>0.01263301303279465</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.1538955599782551</v>
+        <v>0.003060069330086296</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.1167778975350871</v>
+        <v>0.0006353438032756793</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.07753597755069662</v>
+        <v>0.0001154235383960217</v>
       </c>
       <c r="AM11" t="n">
-        <v>0.04576077373573061</v>
+        <v>1.863920765372472e-05</v>
       </c>
       <c r="AN11" t="n">
-        <v>0.02430669775680833</v>
+        <v>2.708962661411352e-06</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.01173723709013715</v>
+        <v>3.579199501128622e-07</v>
       </c>
       <c r="AP11" t="n">
-        <v>0.005195378981452911</v>
+        <v>4.334911470142355e-08</v>
       </c>
       <c r="AQ11" t="n">
-        <v>0.002122787308615934</v>
+        <v>4.846324079245526e-09</v>
       </c>
       <c r="AR11" t="n">
-        <v>0.0008053989304478993</v>
+        <v>5.031065705180462e-10</v>
       </c>
       <c r="AS11" t="n">
-        <v>0.0002852018847570036</v>
+        <v>4.8746596942807e-11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>